<commit_message>
Java 17 First UT/IT \o/
</commit_message>
<xml_diff>
--- a/src/test/resources/drinkData.xlsx
+++ b/src/test/resources/drinkData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="drinks" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="201">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -470,10 +470,28 @@
     <t xml:space="preserve">replaceByName</t>
   </si>
   <si>
+    <t xml:space="preserve">Bière de froment / Blanche</t>
+  </si>
+  <si>
     <t xml:space="preserve">Minérale</t>
   </si>
   <si>
+    <t xml:space="preserve">IPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bière de fermentation basse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lambic/Bière acide</t>
+  </si>
+  <si>
     <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triple Wet Hopped Kölsch</t>
   </si>
   <si>
     <t xml:space="preserve">Couleur dorée et généralement limpide</t>
@@ -618,11 +636,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -644,12 +663,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -695,7 +708,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -705,10 +718,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -731,11 +740,11 @@
   </sheetPr>
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2637,15 +2646,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2673,199 +2682,94 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1569</v>
+        <v>1574</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>1587</v>
+        <v>1576</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>1580</v>
+        <v>1585</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>1586</v>
+        <v>1588</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>151</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>1574</v>
+        <v>1567</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>1576</v>
+        <v>1582</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>148</v>
+        <v>59</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>118</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>1576</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>1579</v>
-      </c>
       <c r="B9" s="2" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>1585</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>1588</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>1567</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>1582</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>148</v>
-      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>1573</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>1577</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>1589</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>1568</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>1583</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>1576</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>1571</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>1575</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>1578</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>1572</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>1581</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>1570</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="B14" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2883,13 +2787,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2915,13 +2819,13 @@
       <c r="A2" s="0" t="n">
         <v>1564</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" s="3" t="n">
+      <c r="D2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>1562</v>
       </c>
     </row>
@@ -2929,65 +2833,71 @@
       <c r="A3" s="0" t="n">
         <v>1563</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>150</v>
+      <c r="C3" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1565</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>151</v>
+      <c r="C4" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1562</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>153</v>
+      <c r="B5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1566</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>155</v>
+      <c r="B6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>1561</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>156</v>
+      <c r="C7" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
+      <c r="B8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3010,7 +2920,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3020,10 +2930,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>10</v>
@@ -3043,10 +2953,10 @@
         <v>49</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3057,10 +2967,10 @@
         <v>140</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3071,10 +2981,10 @@
         <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3085,10 +2995,10 @@
         <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3099,10 +3009,10 @@
         <v>34</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3113,10 +3023,10 @@
         <v>47</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3127,10 +3037,10 @@
         <v>52</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3141,10 +3051,10 @@
         <v>12</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3155,10 +3065,10 @@
         <v>83</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3169,10 +3079,10 @@
         <v>136</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3183,10 +3093,10 @@
         <v>143</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,10 +3107,10 @@
         <v>56</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3211,10 +3121,10 @@
         <v>37</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,10 +3135,10 @@
         <v>45</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3239,10 +3149,10 @@
         <v>72</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3253,10 +3163,10 @@
         <v>61</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3267,10 +3177,10 @@
         <v>70</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3281,10 +3191,10 @@
         <v>77</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3295,10 +3205,10 @@
         <v>63</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3309,10 +3219,10 @@
         <v>79</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3323,10 +3233,10 @@
         <v>16</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3337,10 +3247,10 @@
         <v>98</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3351,10 +3261,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,10 +3275,10 @@
         <v>90</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3379,10 +3289,10 @@
         <v>93</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3393,10 +3303,10 @@
         <v>95</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3407,10 +3317,10 @@
         <v>138</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3421,10 +3331,10 @@
         <v>108</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3435,10 +3345,10 @@
         <v>111</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3449,10 +3359,10 @@
         <v>113</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3463,10 +3373,10 @@
         <v>123</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3477,10 +3387,10 @@
         <v>128</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3491,10 +3401,10 @@
         <v>74</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3505,10 +3415,10 @@
         <v>130</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,10 +3429,10 @@
         <v>132</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3533,10 +3443,10 @@
         <v>134</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3547,10 +3457,10 @@
         <v>66</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3575,7 +3485,7 @@
       <selection pane="topLeft" activeCell="P16" activeCellId="0" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3585,10 +3495,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>10</v>
@@ -3605,10 +3515,10 @@
         <v>1618</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>183</v>
+        <v>170</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3616,10 +3526,10 @@
         <v>1616</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>184</v>
+        <v>172</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3627,10 +3537,10 @@
         <v>1594</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>185</v>
+        <v>168</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3638,16 +3548,16 @@
         <v>1590</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3655,10 +3565,10 @@
         <v>1600</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>188</v>
+        <v>176</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3666,10 +3576,10 @@
         <v>1592</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3677,10 +3587,10 @@
         <v>1609</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3688,10 +3598,10 @@
         <v>1603</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>191</v>
+        <v>180</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3699,10 +3609,10 @@
         <v>1625</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>192</v>
+        <v>178</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3710,18 +3620,18 @@
         <v>1597</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>193</v>
+        <v>174</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>